<commit_message>
update 2019Q2 report with figs by year only, altered axis text size
</commit_message>
<xml_diff>
--- a/data/Research_Metrics.xlsx
+++ b/data/Research_Metrics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22019"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_3e87\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="308" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{F9AE7A8B-B779-4E26-A9E8-72684F44291E}"/>
+  <xr:revisionPtr revIDLastSave="310" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D8DC34E9-AED7-42FA-BECE-288D4804633C}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="158">
   <si>
     <t>SubmissionTime</t>
   </si>
@@ -609,8 +609,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5BDB1E2E-CB32-46E7-93A5-00BC09511A10}" name="Table1" displayName="Table1" ref="A1:G143" totalsRowShown="0">
-  <autoFilter ref="A1:G143" xr:uid="{D097265D-4419-449A-8945-3B1FC2CD4B71}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5BDB1E2E-CB32-46E7-93A5-00BC09511A10}" name="Table1" displayName="Table1" ref="A1:G145" totalsRowShown="0">
+  <autoFilter ref="A1:G145" xr:uid="{D097265D-4419-449A-8945-3B1FC2CD4B71}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -932,10 +932,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G143"/>
+  <dimension ref="A1:G145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="F135" sqref="F135"/>
+    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="A146" sqref="A146:XFD146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3681,6 +3681,46 @@
       </c>
       <c r="G143" t="s">
         <v>157</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7">
+      <c r="A144" s="1">
+        <v>43634.724305555559</v>
+      </c>
+      <c r="B144" t="s">
+        <v>77</v>
+      </c>
+      <c r="C144" t="s">
+        <v>10</v>
+      </c>
+      <c r="D144" s="2">
+        <v>43564</v>
+      </c>
+      <c r="F144">
+        <v>20</v>
+      </c>
+      <c r="G144" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7">
+      <c r="A145" s="1">
+        <v>43634.724999999999</v>
+      </c>
+      <c r="B145" t="s">
+        <v>77</v>
+      </c>
+      <c r="C145" t="s">
+        <v>10</v>
+      </c>
+      <c r="D145" s="2">
+        <v>43565</v>
+      </c>
+      <c r="F145">
+        <v>19</v>
+      </c>
+      <c r="G145" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -3701,15 +3741,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010016563BE3E692244C851CEBE22D8D3059" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f18de4ed1ecee09398aaa4953f2d63e2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="5518ca6b-e5cc-490e-b98e-d5e5b111277c" xmlns:ns3="c1033f61-e676-4180-b03d-6fcaed56d122" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="347e25aa0090c5fa800c70ebe7b93ba0" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3943,6 +3974,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3953,11 +3993,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E31C3F3E-2F8F-4F18-A348-FE85FB0B4FE5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CEA7423-1812-4AEE-AC53-852A91A5C242}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CEA7423-1812-4AEE-AC53-852A91A5C242}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E31C3F3E-2F8F-4F18-A348-FE85FB0B4FE5}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
change several cit/stake engagements to conf/active mtgs
</commit_message>
<xml_diff>
--- a/data/Research_Metrics.xlsx
+++ b/data/Research_Metrics.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22223"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_a74\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="393" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0996E355-9241-4C3A-8A74-B0BD89810A11}"/>
+  <xr:revisionPtr revIDLastSave="410" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A8A61F28-C3E1-423A-A1DB-E0E3B036078B}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="231">
   <si>
     <t>SubmissionTime</t>
   </si>
@@ -719,6 +719,9 @@
   </si>
   <si>
     <t>8 field volunteers in this summer (July to September).</t>
+  </si>
+  <si>
+    <t>McIlroy, SE, Cunning, R, Baker, AC, Coffroth, MA. Competition and succession among coral endosymbionts. Ecol Evol. 2019; 00: 1– 12. https://doi.org/10.1002/ece3.5749</t>
   </si>
 </sst>
 </file>
@@ -825,16 +828,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5BDB1E2E-CB32-46E7-93A5-00BC09511A10}" name="Table1" displayName="Table1" ref="A1:G212" totalsRowShown="0">
-  <autoFilter ref="A1:G212" xr:uid="{D097265D-4419-449A-8945-3B1FC2CD4B71}">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-    <filterColumn colId="6" hiddenButton="1"/>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5BDB1E2E-CB32-46E7-93A5-00BC09511A10}" name="Table1" displayName="Table1" ref="A1:G213" totalsRowShown="0">
+  <autoFilter ref="A1:G213" xr:uid="{D097265D-4419-449A-8945-3B1FC2CD4B71}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G118">
     <sortCondition ref="A1:A118"/>
   </sortState>
@@ -1148,10 +1143,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G212"/>
+  <dimension ref="A1:G213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="E150" sqref="E150"/>
+    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
+      <selection activeCell="D210" sqref="D210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2382,7 +2377,7 @@
         <v>77</v>
       </c>
       <c r="C64" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D64" s="2">
         <v>43565</v>
@@ -2479,7 +2474,7 @@
         <v>77</v>
       </c>
       <c r="C69" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D69" s="2">
         <v>43564</v>
@@ -2499,7 +2494,7 @@
         <v>77</v>
       </c>
       <c r="C70" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D70" s="2">
         <v>43565</v>
@@ -2519,7 +2514,7 @@
         <v>77</v>
       </c>
       <c r="C71" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D71" s="2">
         <v>43568</v>
@@ -3365,7 +3360,7 @@
         <v>120</v>
       </c>
       <c r="C116" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D116" s="2">
         <v>43530</v>
@@ -3385,7 +3380,7 @@
         <v>120</v>
       </c>
       <c r="C117" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D117" s="2">
         <v>43529</v>
@@ -3619,7 +3614,7 @@
         <v>7</v>
       </c>
       <c r="C129" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D129" s="2">
         <v>43649</v>
@@ -3950,7 +3945,7 @@
         <v>7</v>
       </c>
       <c r="C146" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D146" s="2">
         <v>43705</v>
@@ -3970,7 +3965,7 @@
         <v>20</v>
       </c>
       <c r="C147" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D147" s="2">
         <v>43706</v>
@@ -4447,7 +4442,7 @@
         <v>26</v>
       </c>
       <c r="C171" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D171" s="2">
         <v>43718</v>
@@ -4664,7 +4659,7 @@
         <v>120</v>
       </c>
       <c r="C182" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D182" s="2">
         <v>43754</v>
@@ -4704,7 +4699,7 @@
         <v>20</v>
       </c>
       <c r="C184" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D184" s="2">
         <v>43756</v>
@@ -4824,7 +4819,7 @@
         <v>40</v>
       </c>
       <c r="C190" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D190" s="2">
         <v>43761</v>
@@ -5015,7 +5010,7 @@
         <v>7</v>
       </c>
       <c r="C200" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D200" s="2">
         <v>43704</v>
@@ -5212,7 +5207,7 @@
         <v>40</v>
       </c>
       <c r="C210" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D210" s="2">
         <v>43677</v>
@@ -5262,6 +5257,23 @@
       </c>
       <c r="G212" t="s">
         <v>229</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7">
+      <c r="A213" s="1">
+        <v>43768.587094907409</v>
+      </c>
+      <c r="B213" t="s">
+        <v>7</v>
+      </c>
+      <c r="C213" t="s">
+        <v>15</v>
+      </c>
+      <c r="D213" s="2">
+        <v>43767</v>
+      </c>
+      <c r="E213" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -5285,24 +5297,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010016563BE3E692244C851CEBE22D8D3059" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f18de4ed1ecee09398aaa4953f2d63e2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="5518ca6b-e5cc-490e-b98e-d5e5b111277c" xmlns:ns3="c1033f61-e676-4180-b03d-6fcaed56d122" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="347e25aa0090c5fa800c70ebe7b93ba0" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5536,14 +5530,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CEA7423-1812-4AEE-AC53-852A91A5C242}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59E6B255-4F2B-419A-A912-00D5A9DAB81B}"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E31C3F3E-2F8F-4F18-A348-FE85FB0B4FE5}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CEA7423-1812-4AEE-AC53-852A91A5C242}"/>
 </file>
</xml_diff>

<commit_message>
change some stakeholders to presentations
</commit_message>
<xml_diff>
--- a/data/Research_Metrics.xlsx
+++ b/data/Research_Metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_a74\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="440" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3654D689-E397-4A9A-A0DE-BC1356D542E4}"/>
+  <xr:revisionPtr revIDLastSave="457" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{135B755E-3983-4160-9F57-2D7EF3945C6D}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="265">
   <si>
     <t>SubmissionTime</t>
   </si>
@@ -817,6 +817,15 @@
   </si>
   <si>
     <t>van den Burg, M.P., Brisbane, J.L.K. &amp; Knapp, C.R. Biol Invasions (2019). https://doi.org/10.1007/s10530-019-02107-5</t>
+  </si>
+  <si>
+    <t>http://iaglr.org/ll/2019-3-Fall_LL3.pdf</t>
+  </si>
+  <si>
+    <t>Non-peer reviewed publication I wrote about how the black spot disease paper came to be. Also speaks on Great Lakes Fish Finder and iNaturalist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haerther Work Day - buckthorn removal </t>
   </si>
 </sst>
 </file>
@@ -923,8 +932,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5BDB1E2E-CB32-46E7-93A5-00BC09511A10}" name="Table1" displayName="Table1" ref="A1:G239" totalsRowShown="0">
-  <autoFilter ref="A1:G239" xr:uid="{D097265D-4419-449A-8945-3B1FC2CD4B71}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5BDB1E2E-CB32-46E7-93A5-00BC09511A10}" name="Table1" displayName="Table1" ref="A1:G241" totalsRowShown="0">
+  <autoFilter ref="A1:G241" xr:uid="{D097265D-4419-449A-8945-3B1FC2CD4B71}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{257521A4-A155-4B02-A306-C59860E67EED}" name="SubmissionTime"/>
     <tableColumn id="2" xr3:uid="{37A5D46C-63FC-4A5A-BC50-C4BE807BE242}" name="ResponderEmail"/>
@@ -1235,10 +1244,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G239"/>
+  <dimension ref="A1:G241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A225" workbookViewId="0">
-      <selection activeCell="E239" sqref="E239"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C172" sqref="C172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3977,7 +3986,7 @@
         <v>77</v>
       </c>
       <c r="C143" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D143" s="2">
         <v>43564</v>
@@ -3997,7 +4006,7 @@
         <v>77</v>
       </c>
       <c r="C144" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D144" s="2">
         <v>43565</v>
@@ -4971,7 +4980,7 @@
         <v>120</v>
       </c>
       <c r="C193" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D193" s="2">
         <v>43763</v>
@@ -5396,7 +5405,7 @@
         <v>120</v>
       </c>
       <c r="C215" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D215" s="2">
         <v>43773</v>
@@ -5416,7 +5425,7 @@
         <v>120</v>
       </c>
       <c r="C216" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D216" s="2">
         <v>43768</v>
@@ -5436,7 +5445,7 @@
         <v>20</v>
       </c>
       <c r="C217" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D217" s="2">
         <v>43776</v>
@@ -5456,7 +5465,7 @@
         <v>77</v>
       </c>
       <c r="C218" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D218" s="2">
         <v>43777</v>
@@ -5856,6 +5865,46 @@
       </c>
       <c r="E239" t="s">
         <v>261</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7">
+      <c r="A240" s="1">
+        <v>43818.635567129626</v>
+      </c>
+      <c r="B240" t="s">
+        <v>20</v>
+      </c>
+      <c r="C240" t="s">
+        <v>28</v>
+      </c>
+      <c r="D240" s="2">
+        <v>43790</v>
+      </c>
+      <c r="E240" t="s">
+        <v>262</v>
+      </c>
+      <c r="G240" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="241" spans="1:7">
+      <c r="A241" s="1">
+        <v>43818.636030092595</v>
+      </c>
+      <c r="B241" t="s">
+        <v>20</v>
+      </c>
+      <c r="C241" t="s">
+        <v>8</v>
+      </c>
+      <c r="D241" s="2">
+        <v>43817</v>
+      </c>
+      <c r="F241">
+        <v>1</v>
+      </c>
+      <c r="G241" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -5888,15 +5937,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010016563BE3E692244C851CEBE22D8D3059" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f18de4ed1ecee09398aaa4953f2d63e2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="5518ca6b-e5cc-490e-b98e-d5e5b111277c" xmlns:ns3="c1033f61-e676-4180-b03d-6fcaed56d122" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="347e25aa0090c5fa800c70ebe7b93ba0" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6130,14 +6170,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E31C3F3E-2F8F-4F18-A348-FE85FB0B4FE5}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59E6B255-4F2B-419A-A912-00D5A9DAB81B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CEA7423-1812-4AEE-AC53-852A91A5C242}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CEA7423-1812-4AEE-AC53-852A91A5C242}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59E6B255-4F2B-419A-A912-00D5A9DAB81B}"/>
 </file>
</xml_diff>

<commit_message>
run 2019 final report
</commit_message>
<xml_diff>
--- a/data/Research_Metrics.xlsx
+++ b/data/Research_Metrics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22505"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_a74\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C291A9A-0D2F-4AA2-AAF2-7A9762333CBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{15F2695F-3AE6-4DD4-9D82-5765F6E22671}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="288">
   <si>
     <t>SubmissionTime</t>
   </si>
@@ -865,6 +865,36 @@
   </si>
   <si>
     <t xml:space="preserve">Buckthorn removal </t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/MicroFishing/comments/elty76/rmicrofishing_shout_out_in_research_paper/</t>
+  </si>
+  <si>
+    <t>Posted to the Reddit Microfishing page that we spoke about them in a research paper. It received 50 upvotes, which means ATLEAST 50 people read my post, but likely way more did as the community numbers &gt; 5,000</t>
+  </si>
+  <si>
+    <t>Lecture and Lab for vertebrate ecology course at Loyola.</t>
+  </si>
+  <si>
+    <t>Inoue K, Pohl AL, Makiri S, Lang BK, Berg DJ. (2020) Use of species delimitation approach to assess biodiversity in freshwater planarians (Platyhelminthes: Tricladida) from desert springs. Aquatic Conservation: Marine and Freshwater Ecosystems, DOI: 10.1002/aqc.3273</t>
+  </si>
+  <si>
+    <t>Presented at The Night of Ideas. &gt;5,000 attended event, and estimated 125 came to my talk.</t>
+  </si>
+  <si>
+    <t>Spoke about our research programs at the 'Waves of Gratitude' event for the auxiliary board</t>
+  </si>
+  <si>
+    <t>Coral research trip</t>
+  </si>
+  <si>
+    <t>Coral trip</t>
+  </si>
+  <si>
+    <t>Interview for ScienceWorld - a Scholastic magazine for highschoolers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Happel A., K.J. Murchie, P. W. Willink, and C.R. Knapp. In Press. Great Lakes Fish Finder App; a tool for biologists, managers and education practitioners. Journal of Great Lakes Research. XX:XX-XX. https://doi.org/10.1016/j.jglr.2019.12.002 </t>
   </si>
 </sst>
 </file>
@@ -971,8 +1001,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5BDB1E2E-CB32-46E7-93A5-00BC09511A10}" name="Table1" displayName="Table1" ref="A1:G252" totalsRowShown="0">
-  <autoFilter ref="A1:G252" xr:uid="{D097265D-4419-449A-8945-3B1FC2CD4B71}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5BDB1E2E-CB32-46E7-93A5-00BC09511A10}" name="Table1" displayName="Table1" ref="A1:G261" totalsRowShown="0">
+  <autoFilter ref="A1:G261" xr:uid="{D097265D-4419-449A-8945-3B1FC2CD4B71}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{257521A4-A155-4B02-A306-C59860E67EED}" name="SubmissionTime"/>
     <tableColumn id="2" xr3:uid="{37A5D46C-63FC-4A5A-BC50-C4BE807BE242}" name="ResponderEmail"/>
@@ -1283,10 +1313,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G252"/>
+  <dimension ref="A1:G261"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
-      <selection activeCell="F245" sqref="F245"/>
+    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
+      <selection activeCell="F251" sqref="F251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6120,7 +6150,7 @@
         <v>43831</v>
       </c>
       <c r="F250">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G250" t="s">
         <v>275</v>
@@ -6164,6 +6194,180 @@
       </c>
       <c r="G252" t="s">
         <v>277</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7">
+      <c r="A253" s="1">
+        <v>43843.74900462963</v>
+      </c>
+      <c r="B253" t="s">
+        <v>20</v>
+      </c>
+      <c r="C253" t="s">
+        <v>10</v>
+      </c>
+      <c r="D253" s="2">
+        <v>43838</v>
+      </c>
+      <c r="E253" t="s">
+        <v>278</v>
+      </c>
+      <c r="F253">
+        <v>50</v>
+      </c>
+      <c r="G253" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="254" spans="1:7">
+      <c r="A254" s="1">
+        <v>43858.879895833335</v>
+      </c>
+      <c r="B254" t="s">
+        <v>20</v>
+      </c>
+      <c r="C254" t="s">
+        <v>10</v>
+      </c>
+      <c r="D254" s="2">
+        <v>43852</v>
+      </c>
+      <c r="F254">
+        <v>15</v>
+      </c>
+      <c r="G254" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="255" spans="1:7">
+      <c r="A255" s="1">
+        <v>43859.769270833334</v>
+      </c>
+      <c r="B255" t="s">
+        <v>40</v>
+      </c>
+      <c r="C255" t="s">
+        <v>15</v>
+      </c>
+      <c r="D255" s="2">
+        <v>43852</v>
+      </c>
+      <c r="E255" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="256" spans="1:7">
+      <c r="A256" s="1">
+        <v>43861.711574074077</v>
+      </c>
+      <c r="B256" t="s">
+        <v>20</v>
+      </c>
+      <c r="C256" t="s">
+        <v>10</v>
+      </c>
+      <c r="D256" s="2">
+        <v>43860</v>
+      </c>
+      <c r="F256">
+        <v>125</v>
+      </c>
+      <c r="G256" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="257" spans="1:7">
+      <c r="A257" s="1">
+        <v>43861.778101851851</v>
+      </c>
+      <c r="B257" t="s">
+        <v>111</v>
+      </c>
+      <c r="C257" t="s">
+        <v>10</v>
+      </c>
+      <c r="D257" s="2">
+        <v>43790</v>
+      </c>
+      <c r="F257">
+        <v>50</v>
+      </c>
+      <c r="G257" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="258" spans="1:7">
+      <c r="A258" s="1">
+        <v>43861.778796296298</v>
+      </c>
+      <c r="B258" t="s">
+        <v>111</v>
+      </c>
+      <c r="C258" t="s">
+        <v>8</v>
+      </c>
+      <c r="D258" s="2">
+        <v>43743</v>
+      </c>
+      <c r="F258">
+        <v>7</v>
+      </c>
+      <c r="G258" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="259" spans="1:7">
+      <c r="A259" s="1">
+        <v>43861.779282407406</v>
+      </c>
+      <c r="B259" t="s">
+        <v>77</v>
+      </c>
+      <c r="C259" t="s">
+        <v>8</v>
+      </c>
+      <c r="D259" s="2">
+        <v>43749</v>
+      </c>
+      <c r="F259">
+        <v>7</v>
+      </c>
+      <c r="G259" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="260" spans="1:7">
+      <c r="A260" s="1">
+        <v>43861.779849537037</v>
+      </c>
+      <c r="B260" t="s">
+        <v>77</v>
+      </c>
+      <c r="C260" t="s">
+        <v>28</v>
+      </c>
+      <c r="D260" s="2">
+        <v>43861</v>
+      </c>
+      <c r="G260" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="261" spans="1:7">
+      <c r="A261" s="1">
+        <v>43861.918692129628</v>
+      </c>
+      <c r="B261" t="s">
+        <v>26</v>
+      </c>
+      <c r="C261" t="s">
+        <v>15</v>
+      </c>
+      <c r="D261" s="2">
+        <v>43826</v>
+      </c>
+      <c r="E261" t="s">
+        <v>287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20200831 update with fixed data
</commit_message>
<xml_diff>
--- a/data/Research_Metrics.xlsx
+++ b/data/Research_Metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sheddaquarium.sharepoint.com/sites/Conservation/Shared Documents/Files/Research/Quarterly metrics for Conservation Research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{14861805-1095-4379-B365-CB54576F7BC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{74A3962A-AE00-41F8-8424-297717E20809}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="27380" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="448">
   <si>
     <t>SubmissionTime</t>
   </si>
@@ -435,6 +435,9 @@
   </si>
   <si>
     <t>Pedro, S., Fisk, A. T., Ferguson, S. H., Hussey, N. E., Kessel, S. T., &amp; McKinney, M. A. (2019). Limited effects of changing prey fish communities on food quality for aquatic predators in the eastern Canadian Arctic in terms of essential fatty acids, methylmercury and selenium. Chemosphere, 214, 855-865.</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/full/10.1111/ddi.12860</t>
   </si>
   <si>
     <t>Yurkowski, D. J., Auger_Méthé, M., Mallory, M. L., Wong, S. N., Gilchrist, G., Derocher, A. E., ... &amp; Togunov, R. R. (2018). Abundance and species diversity hotspots of tracked marine predators across the North American Arctic. Diversity and Distributions.</t>
@@ -858,7 +861,8 @@
     <t>IUCN Iguana Specialist Group meeting</t>
   </si>
   <si>
-    <t>van den Burg, M.P., Brisbane, J.L.K. &amp; Knapp, C.R. Biol Invasions (2019). https://doi.org/10.1007/s10530-019-02107-5</t>
+    <t xml:space="preserve">Van den Burg, M. P., Brisbane, J. L., &amp; Knapp, C. R. (2020). Post-hurricane relief facilitates invasion and establishment of two invasive alien vertebrate species in the Commonwealth of Dominica, West Indies. Biological Invasions, 22(2), 195–203. https://doi.org/10.1007/s10530-019-02107-5
+</t>
   </si>
   <si>
     <t>http://iaglr.org/ll/2019-3-Fall_LL3.pdf</t>
@@ -936,7 +940,7 @@
     <t>Interview for ScienceWorld - a Scholastic magazine for highschoolers</t>
   </si>
   <si>
-    <t xml:space="preserve">Happel A., K.J. Murchie, P. W. Willink, and C.R. Knapp. In Press. Great Lakes Fish Finder App; a tool for biologists, managers and education practitioners. Journal of Great Lakes Research. XX:XX-XX. https://doi.org/10.1016/j.jglr.2019.12.002 </t>
+    <t>Happel A., Murchie, K. J., Willink, P. W., &amp; Knapp, C. R. (2020). Great Lakes Fish Finder App; a tool for biologists, managers and education practitioners. Journal of Great Lakes Research, 46(1), 230-236. https://doi.org/10.1016/j.jglr.2019.12.002</t>
   </si>
   <si>
     <t>Q&amp;A at 'Chasing Coral' screening at Downer's Grove public library</t>
@@ -957,7 +961,10 @@
     <t>Weeks, C, Meagher, S, Willink, P, McCravy, KW. Does seawater acidification affect zooxanthellae density and health in the invasive upside‐down jellyfish, Cassiopea spp.? Invertebr Biol. 2019; 138:e12255. https://doi.org/10.1111/ivb.12255</t>
   </si>
   <si>
-    <t>Lynn Waterhouse, Scott A. Heppell, Christy V. Pattengill-Semmens, Croy McCoy, Phillippe Bush, Bradley C. Johnson, Brice X. Semmens Proceedings of the National Academy of Sciences Jan 2020, 117 (3) 1587-1595; DOI: 10.1073/pnas.1917132117</t>
+    <t>https://www.pnas.org/content/117/3/1587/tab-article-info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waterhouse, L., Heppell, S. A., Pattengill-Semmens, C. V., McCoy, C., Bush, P., Johnson, B. C., and Semmens, B. X. (2020). Recovery of critically endangered Nassau grouper (Epinephelus striatus) in the Cayman Islands following targeted conservation actions. Proceedings of the National Academy of Sciences, 117(3), 1587-1595. https://doi.org/10.1073/pnas.1917132117 </t>
   </si>
   <si>
     <t>PNAS paper - legacy project on Cayman grouper. Technically print date is 2020.</t>
@@ -1420,6 +1427,12 @@
   </si>
   <si>
     <t>Interview about collaborative research with University of Windsor tagging yellow perch with transmitters that change signal following a predation event</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S2213224419300999</t>
+  </si>
+  <si>
+    <t>Happel, A. (2019). A volunteer-populated online database provides evidence for a geographic pattern in symptoms of black spot infections. International Journal for Parasitology: Parasites and Wildlife, 10, 156-163. https://doi.org/10.1016/j.ijppaw.2019.08.003</t>
   </si>
 </sst>
 </file>
@@ -1494,7 +1507,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1510,6 +1523,7 @@
     <xf numFmtId="22" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1545,8 +1559,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5BDB1E2E-CB32-46E7-93A5-00BC09511A10}" name="Table1" displayName="Table1" ref="A1:I379" totalsRowShown="0">
-  <autoFilter ref="A1:I379" xr:uid="{D097265D-4419-449A-8945-3B1FC2CD4B71}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5BDB1E2E-CB32-46E7-93A5-00BC09511A10}" name="Table1" displayName="Table1" ref="A1:I380" totalsRowShown="0">
+  <autoFilter ref="A1:I380" xr:uid="{D097265D-4419-449A-8945-3B1FC2CD4B71}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I374">
     <sortCondition ref="A2:A374"/>
   </sortState>
@@ -1914,10 +1928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I379"/>
+  <dimension ref="A1:I380"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A364" workbookViewId="0">
-      <selection activeCell="A379" sqref="A379:XFD379"/>
+    <sheetView tabSelected="1" topLeftCell="C163" workbookViewId="0">
+      <selection activeCell="E164" sqref="E164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -3899,9 +3913,11 @@
       <c r="D98" s="2">
         <v>43500</v>
       </c>
-      <c r="E98" s="2"/>
+      <c r="E98" s="13" t="s">
+        <v>116</v>
+      </c>
       <c r="F98" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -3922,7 +3938,7 @@
         <v>100</v>
       </c>
       <c r="I99" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="100" spans="1:9">
@@ -3943,7 +3959,7 @@
         <v>30</v>
       </c>
       <c r="I100" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="101" spans="1:9">
@@ -3964,7 +3980,7 @@
         <v>200</v>
       </c>
       <c r="I101" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="102" spans="1:9">
@@ -3981,7 +3997,7 @@
         <v>43572</v>
       </c>
       <c r="E102" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="103" spans="1:9">
@@ -4038,7 +4054,7 @@
         <v>12</v>
       </c>
       <c r="I105" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="106" spans="1:9">
@@ -4059,7 +4075,7 @@
         <v>7</v>
       </c>
       <c r="I106" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="107" spans="1:9">
@@ -4067,7 +4083,7 @@
         <v>43637.12096064815</v>
       </c>
       <c r="B107" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C107" t="s">
         <v>12</v>
@@ -4077,7 +4093,7 @@
       </c>
       <c r="E107" s="2"/>
       <c r="I107" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="108" spans="1:9">
@@ -4085,7 +4101,7 @@
         <v>43637.125092592592</v>
       </c>
       <c r="B108" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C108" t="s">
         <v>28</v>
@@ -4094,10 +4110,10 @@
         <v>43571</v>
       </c>
       <c r="E108" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I108" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="109" spans="1:9">
@@ -4105,7 +4121,7 @@
         <v>43637.126643518517</v>
       </c>
       <c r="B109" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C109" t="s">
         <v>10</v>
@@ -4118,7 +4134,7 @@
         <v>18</v>
       </c>
       <c r="I109" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="110" spans="1:9">
@@ -4126,7 +4142,7 @@
         <v>43637.130104166667</v>
       </c>
       <c r="B110" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C110" t="s">
         <v>12</v>
@@ -4136,7 +4152,7 @@
       </c>
       <c r="E110" s="2"/>
       <c r="I110" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="111" spans="1:9">
@@ -4144,7 +4160,7 @@
         <v>43637.130798611113</v>
       </c>
       <c r="B111" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C111" t="s">
         <v>12</v>
@@ -4154,7 +4170,7 @@
       </c>
       <c r="E111" s="2"/>
       <c r="I111" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="112" spans="1:9">
@@ -4162,7 +4178,7 @@
         <v>43637.132118055553</v>
       </c>
       <c r="B112" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C112" t="s">
         <v>12</v>
@@ -4175,7 +4191,7 @@
         <v>5</v>
       </c>
       <c r="I112" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="113" spans="1:9">
@@ -4183,7 +4199,7 @@
         <v>43637.132731481484</v>
       </c>
       <c r="B113" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C113" t="s">
         <v>12</v>
@@ -4193,7 +4209,7 @@
       </c>
       <c r="E113" s="2"/>
       <c r="I113" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="114" spans="1:9">
@@ -4201,7 +4217,7 @@
         <v>43637.134652777779</v>
       </c>
       <c r="B114" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C114" t="s">
         <v>12</v>
@@ -4211,7 +4227,7 @@
       </c>
       <c r="E114" s="2"/>
       <c r="I114" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="115" spans="1:9">
@@ -4219,7 +4235,7 @@
         <v>43637.135844907411</v>
       </c>
       <c r="B115" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C115" t="s">
         <v>10</v>
@@ -4232,7 +4248,7 @@
         <v>9</v>
       </c>
       <c r="I115" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="116" spans="1:9">
@@ -4240,7 +4256,7 @@
         <v>43637.13658564815</v>
       </c>
       <c r="B116" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C116" t="s">
         <v>12</v>
@@ -4250,7 +4266,7 @@
       </c>
       <c r="E116" s="2"/>
       <c r="I116" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="117" spans="1:9">
@@ -4258,7 +4274,7 @@
         <v>43637.138483796298</v>
       </c>
       <c r="B117" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C117" t="s">
         <v>12</v>
@@ -4268,7 +4284,7 @@
       </c>
       <c r="E117" s="2"/>
       <c r="I117" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="118" spans="1:9">
@@ -4276,7 +4292,7 @@
         <v>43637.140381944446</v>
       </c>
       <c r="B118" s="11" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C118" t="s">
         <v>12</v>
@@ -4286,7 +4302,7 @@
       </c>
       <c r="E118" s="2"/>
       <c r="I118" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="119" spans="1:9">
@@ -4294,7 +4310,7 @@
         <v>43637.14329861111</v>
       </c>
       <c r="B119" s="14" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C119" t="s">
         <v>10</v>
@@ -4315,7 +4331,7 @@
         <v>43637.14329861111</v>
       </c>
       <c r="B120" s="11" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C120" t="s">
         <v>12</v>
@@ -4325,7 +4341,7 @@
       </c>
       <c r="E120" s="2"/>
       <c r="I120" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="121" spans="1:9">
@@ -4354,7 +4370,7 @@
         <v>43643.14329861111</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C122" t="s">
         <v>10</v>
@@ -4367,7 +4383,7 @@
         <v>1</v>
       </c>
       <c r="I122" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="123" spans="1:9">
@@ -4388,7 +4404,7 @@
         <v>1</v>
       </c>
       <c r="I123" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="124" spans="1:9">
@@ -4406,7 +4422,7 @@
       </c>
       <c r="E124" s="2"/>
       <c r="F124" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="125" spans="1:9">
@@ -4427,7 +4443,7 @@
         <v>6</v>
       </c>
       <c r="I125" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="126" spans="1:9">
@@ -4435,7 +4451,7 @@
         <v>43649.622928240744</v>
       </c>
       <c r="B126" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C126" t="s">
         <v>10</v>
@@ -4448,7 +4464,7 @@
         <v>8.5</v>
       </c>
       <c r="I126" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="127" spans="1:9">
@@ -4469,7 +4485,7 @@
         <v>9</v>
       </c>
       <c r="I127" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="128" spans="1:9">
@@ -4487,7 +4503,7 @@
       </c>
       <c r="E128" s="2"/>
       <c r="F128" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="129" spans="1:9">
@@ -4508,7 +4524,7 @@
         <v>5</v>
       </c>
       <c r="I129" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="130" spans="1:9">
@@ -4529,7 +4545,7 @@
         <v>86</v>
       </c>
       <c r="I130" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="131" spans="1:9">
@@ -4550,7 +4566,7 @@
         <v>1</v>
       </c>
       <c r="I131" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="132" spans="1:9">
@@ -4574,7 +4590,7 @@
         <v>50</v>
       </c>
       <c r="I132" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="133" spans="1:9">
@@ -4592,7 +4608,7 @@
       </c>
       <c r="E133" s="2"/>
       <c r="F133" s="9" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="134" spans="1:9">
@@ -4613,7 +4629,7 @@
         <v>1</v>
       </c>
       <c r="I134" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="135" spans="1:9">
@@ -4634,7 +4650,7 @@
         <v>6</v>
       </c>
       <c r="I135" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="136" spans="1:9" ht="14.25" customHeight="1">
@@ -4651,7 +4667,7 @@
         <v>43686</v>
       </c>
       <c r="E136" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="137" spans="1:9">
@@ -4672,7 +4688,7 @@
         <v>200</v>
       </c>
       <c r="I137" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="138" spans="1:9">
@@ -4693,7 +4709,7 @@
         <v>1</v>
       </c>
       <c r="I138" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="139" spans="1:9">
@@ -4717,7 +4733,7 @@
         <v>160</v>
       </c>
       <c r="I139" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="140" spans="1:9">
@@ -4741,7 +4757,7 @@
         <v>320</v>
       </c>
       <c r="I140" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="141" spans="1:9">
@@ -4765,7 +4781,7 @@
         <v>520</v>
       </c>
       <c r="I141" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="142" spans="1:9">
@@ -4789,7 +4805,7 @@
         <v>400</v>
       </c>
       <c r="I142" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="143" spans="1:9">
@@ -4813,7 +4829,7 @@
         <v>480</v>
       </c>
       <c r="I143" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="144" spans="1:9">
@@ -4830,10 +4846,10 @@
         <v>43670</v>
       </c>
       <c r="E144" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I144" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="145" spans="1:9">
@@ -4854,7 +4870,7 @@
         <v>120</v>
       </c>
       <c r="I145" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="146" spans="1:9">
@@ -4875,7 +4891,7 @@
         <v>60</v>
       </c>
       <c r="I146" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="147" spans="1:9">
@@ -4896,7 +4912,7 @@
         <v>5</v>
       </c>
       <c r="I147" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="148" spans="1:9">
@@ -4913,10 +4929,10 @@
         <v>43712</v>
       </c>
       <c r="E148" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I148" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="149" spans="1:9">
@@ -4933,10 +4949,10 @@
         <v>43724</v>
       </c>
       <c r="E149" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="I149" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="150" spans="1:9">
@@ -4953,10 +4969,10 @@
         <v>43714</v>
       </c>
       <c r="E150" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I150" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="151" spans="1:9">
@@ -4973,10 +4989,10 @@
         <v>43726</v>
       </c>
       <c r="E151" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I151" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="152" spans="1:9">
@@ -4997,7 +5013,7 @@
         <v>11</v>
       </c>
       <c r="I152" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="153" spans="1:9">
@@ -5021,7 +5037,7 @@
         <v>50</v>
       </c>
       <c r="I153" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="154" spans="1:9">
@@ -5042,7 +5058,7 @@
         <v>200</v>
       </c>
       <c r="I154" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="155" spans="1:9">
@@ -5063,7 +5079,7 @@
         <v>9</v>
       </c>
       <c r="I155" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="156" spans="1:9">
@@ -5084,7 +5100,7 @@
         <v>8</v>
       </c>
       <c r="I156" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="157" spans="1:9">
@@ -5105,7 +5121,7 @@
         <v>7</v>
       </c>
       <c r="I157" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="158" spans="1:9">
@@ -5126,7 +5142,7 @@
         <v>1</v>
       </c>
       <c r="I158" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="159" spans="1:9">
@@ -5147,7 +5163,7 @@
         <v>1</v>
       </c>
       <c r="I159" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="160" spans="1:9">
@@ -5168,7 +5184,7 @@
         <v>1</v>
       </c>
       <c r="I160" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="161" spans="1:9">
@@ -5189,7 +5205,7 @@
         <v>1</v>
       </c>
       <c r="I161" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="162" spans="1:9">
@@ -5210,7 +5226,7 @@
         <v>1</v>
       </c>
       <c r="I162" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="163" spans="1:9">
@@ -5231,7 +5247,7 @@
         <v>1</v>
       </c>
       <c r="I163" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="164" spans="1:9">
@@ -5249,7 +5265,7 @@
       </c>
       <c r="E164" s="2"/>
       <c r="F164" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="165" spans="1:9">
@@ -5270,7 +5286,7 @@
         <v>35</v>
       </c>
       <c r="I165" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="166" spans="1:9">
@@ -5291,7 +5307,7 @@
         <v>20</v>
       </c>
       <c r="I166" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="167" spans="1:9">
@@ -5312,7 +5328,7 @@
         <v>40</v>
       </c>
       <c r="I167" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="168" spans="1:9">
@@ -5333,7 +5349,7 @@
         <v>4</v>
       </c>
       <c r="I168" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="169" spans="1:9">
@@ -5354,7 +5370,7 @@
         <v>11</v>
       </c>
       <c r="I169" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="170" spans="1:9">
@@ -5375,7 +5391,7 @@
         <v>45</v>
       </c>
       <c r="I170" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="171" spans="1:9">
@@ -5396,7 +5412,7 @@
         <v>20</v>
       </c>
       <c r="I171" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="172" spans="1:9">
@@ -5404,7 +5420,7 @@
         <v>43741.760833333334</v>
       </c>
       <c r="B172" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C172" t="s">
         <v>10</v>
@@ -5417,7 +5433,7 @@
         <v>11</v>
       </c>
       <c r="I172" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="173" spans="1:9">
@@ -5425,7 +5441,7 @@
         <v>43741.76190972222</v>
       </c>
       <c r="B173" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C173" t="s">
         <v>12</v>
@@ -5435,7 +5451,7 @@
       </c>
       <c r="E173" s="2"/>
       <c r="I173" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="174" spans="1:9">
@@ -5443,7 +5459,7 @@
         <v>43741.763113425928</v>
       </c>
       <c r="B174" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C174" t="s">
         <v>10</v>
@@ -5456,7 +5472,7 @@
         <v>8</v>
       </c>
       <c r="I174" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="175" spans="1:9">
@@ -5464,7 +5480,7 @@
         <v>43741.764016203706</v>
       </c>
       <c r="B175" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C175" t="s">
         <v>20</v>
@@ -5474,7 +5490,7 @@
       </c>
       <c r="E175" s="2"/>
       <c r="I175" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="176" spans="1:9">
@@ -5482,7 +5498,7 @@
         <v>43741.765625</v>
       </c>
       <c r="B176" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C176" t="s">
         <v>12</v>
@@ -5492,7 +5508,7 @@
       </c>
       <c r="E176" s="2"/>
       <c r="I176" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="177" spans="1:9">
@@ -5500,7 +5516,7 @@
         <v>43741.767268518517</v>
       </c>
       <c r="B177" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C177" t="s">
         <v>28</v>
@@ -5509,10 +5525,10 @@
         <v>43647</v>
       </c>
       <c r="E177" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I177" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="178" spans="1:9">
@@ -5520,7 +5536,7 @@
         <v>43741.768148148149</v>
       </c>
       <c r="B178" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C178" t="s">
         <v>12</v>
@@ -5530,7 +5546,7 @@
       </c>
       <c r="E178" s="2"/>
       <c r="I178" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="179" spans="1:9">
@@ -5538,7 +5554,7 @@
         <v>43741.770671296297</v>
       </c>
       <c r="B179" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C179" t="s">
         <v>10</v>
@@ -5551,7 +5567,7 @@
         <v>1</v>
       </c>
       <c r="I179" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="180" spans="1:9">
@@ -5576,7 +5592,7 @@
         <v>72</v>
       </c>
       <c r="I180" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="181" spans="1:9">
@@ -5584,7 +5600,7 @@
         <v>43754.878865740742</v>
       </c>
       <c r="B181" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C181" t="s">
         <v>12</v>
@@ -5594,7 +5610,7 @@
       </c>
       <c r="E181" s="2"/>
       <c r="I181" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="182" spans="1:9">
@@ -5615,7 +5631,7 @@
         <v>20</v>
       </c>
       <c r="I182" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="183" spans="1:9">
@@ -5636,7 +5652,7 @@
         <v>40</v>
       </c>
       <c r="I183" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="184" spans="1:9">
@@ -5657,7 +5673,7 @@
         <v>17</v>
       </c>
       <c r="I184" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="185" spans="1:9">
@@ -5681,7 +5697,7 @@
         <v>1232</v>
       </c>
       <c r="I185" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="186" spans="1:9">
@@ -5702,7 +5718,7 @@
         <v>4</v>
       </c>
       <c r="I186" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="187" spans="1:9">
@@ -5723,7 +5739,7 @@
         <v>25</v>
       </c>
       <c r="I187" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="188" spans="1:9">
@@ -5744,7 +5760,7 @@
         <v>4</v>
       </c>
       <c r="I188" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="189" spans="1:9">
@@ -5765,7 +5781,7 @@
         <v>25</v>
       </c>
       <c r="I189" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="190" spans="1:9">
@@ -5786,7 +5802,7 @@
         <v>12</v>
       </c>
       <c r="I190" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="191" spans="1:9">
@@ -5807,7 +5823,7 @@
         <v>25</v>
       </c>
       <c r="I191" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="192" spans="1:9">
@@ -5815,7 +5831,7 @@
         <v>43766.800752314812</v>
       </c>
       <c r="B192" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C192" t="s">
         <v>12</v>
@@ -5825,7 +5841,7 @@
       </c>
       <c r="E192" s="2"/>
       <c r="I192" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="193" spans="1:9">
@@ -5843,7 +5859,7 @@
       </c>
       <c r="E193" s="2"/>
       <c r="I193" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="194" spans="1:9">
@@ -5861,7 +5877,7 @@
       </c>
       <c r="E194" s="2"/>
       <c r="I194" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="195" spans="1:9">
@@ -5878,10 +5894,10 @@
         <v>43754</v>
       </c>
       <c r="E195" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I195" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="196" spans="1:9">
@@ -5889,7 +5905,7 @@
         <v>43766.819953703707</v>
       </c>
       <c r="B196" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C196" t="s">
         <v>12</v>
@@ -5902,7 +5918,7 @@
         <v>1</v>
       </c>
       <c r="I196" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="197" spans="1:9">
@@ -5910,7 +5926,7 @@
         <v>43766.821412037039</v>
       </c>
       <c r="B197" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C197" t="s">
         <v>12</v>
@@ -5920,7 +5936,7 @@
       </c>
       <c r="E197" s="2"/>
       <c r="I197" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="198" spans="1:9">
@@ -5928,7 +5944,7 @@
         <v>43766.822199074071</v>
       </c>
       <c r="B198" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C198" t="s">
         <v>12</v>
@@ -5941,7 +5957,7 @@
         <v>1</v>
       </c>
       <c r="I198" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="199" spans="1:9">
@@ -5962,7 +5978,7 @@
         <v>50</v>
       </c>
       <c r="I199" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="200" spans="1:9">
@@ -5983,7 +5999,7 @@
         <v>30</v>
       </c>
       <c r="I200" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="201" spans="1:9">
@@ -6004,7 +6020,7 @@
         <v>1</v>
       </c>
       <c r="I201" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="202" spans="1:9">
@@ -6025,7 +6041,7 @@
         <v>3</v>
       </c>
       <c r="I202" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="203" spans="1:9">
@@ -6046,7 +6062,7 @@
         <v>4</v>
       </c>
       <c r="I203" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="204" spans="1:9">
@@ -6067,7 +6083,7 @@
         <v>1</v>
       </c>
       <c r="I204" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="205" spans="1:9">
@@ -6088,7 +6104,7 @@
         <v>1</v>
       </c>
       <c r="I205" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="206" spans="1:9">
@@ -6109,7 +6125,7 @@
         <v>1</v>
       </c>
       <c r="I206" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="207" spans="1:9">
@@ -6130,7 +6146,7 @@
         <v>1</v>
       </c>
       <c r="I207" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="208" spans="1:9">
@@ -6148,7 +6164,7 @@
       </c>
       <c r="E208" s="2"/>
       <c r="I208" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="209" spans="1:9">
@@ -6169,7 +6185,7 @@
         <v>25</v>
       </c>
       <c r="I209" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="210" spans="1:9">
@@ -6186,10 +6202,10 @@
         <v>43691</v>
       </c>
       <c r="E210" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="I210" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="211" spans="1:9">
@@ -6210,7 +6226,7 @@
         <v>8</v>
       </c>
       <c r="I211" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="212" spans="1:9">
@@ -6231,7 +6247,7 @@
         <v>14</v>
       </c>
       <c r="I212" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="213" spans="1:9">
@@ -6239,7 +6255,7 @@
         <v>43773.818090277775</v>
       </c>
       <c r="B213" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C213" t="s">
         <v>12</v>
@@ -6249,7 +6265,7 @@
       </c>
       <c r="E213" s="2"/>
       <c r="I213" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="214" spans="1:9">
@@ -6257,7 +6273,7 @@
         <v>43773.819062499999</v>
       </c>
       <c r="B214" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C214" t="s">
         <v>12</v>
@@ -6267,7 +6283,7 @@
       </c>
       <c r="E214" s="2"/>
       <c r="I214" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="215" spans="1:9">
@@ -6288,7 +6304,7 @@
         <v>20</v>
       </c>
       <c r="I215" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="216" spans="1:9">
@@ -6309,7 +6325,7 @@
         <v>23</v>
       </c>
       <c r="I216" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="217" spans="1:9">
@@ -6330,7 +6346,7 @@
         <v>2</v>
       </c>
       <c r="I217" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="218" spans="1:9">
@@ -6351,7 +6367,7 @@
         <v>3</v>
       </c>
       <c r="I218" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="219" spans="1:9">
@@ -6359,7 +6375,7 @@
         <v>43781.848541666666</v>
       </c>
       <c r="B219" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C219" t="s">
         <v>10</v>
@@ -6372,7 +6388,7 @@
         <v>1</v>
       </c>
       <c r="I219" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="220" spans="1:9">
@@ -6393,7 +6409,7 @@
         <v>20</v>
       </c>
       <c r="I220" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="221" spans="1:9">
@@ -6417,7 +6433,7 @@
         <v>120</v>
       </c>
       <c r="I221" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="222" spans="1:9">
@@ -6441,7 +6457,7 @@
         <v>50</v>
       </c>
       <c r="I222" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="223" spans="1:9">
@@ -6459,7 +6475,7 @@
       </c>
       <c r="E223" s="2"/>
       <c r="I223" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="224" spans="1:9">
@@ -6477,7 +6493,7 @@
       </c>
       <c r="E224" s="2"/>
       <c r="I224" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="225" spans="1:9">
@@ -6485,7 +6501,7 @@
         <v>43809.846851851849</v>
       </c>
       <c r="B225" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C225" t="s">
         <v>20</v>
@@ -6498,7 +6514,7 @@
         <v>1</v>
       </c>
       <c r="I225" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="226" spans="1:9">
@@ -6515,10 +6531,10 @@
         <v>43810</v>
       </c>
       <c r="E226" s="5" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="I226" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="227" spans="1:9">
@@ -6535,10 +6551,10 @@
         <v>43810</v>
       </c>
       <c r="E227" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="I227" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="228" spans="1:9">
@@ -6555,10 +6571,10 @@
         <v>43809</v>
       </c>
       <c r="E228" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="I228" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="229" spans="1:9">
@@ -6566,7 +6582,7 @@
         <v>43812.711759259262</v>
       </c>
       <c r="B229" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C229" t="s">
         <v>28</v>
@@ -6575,10 +6591,10 @@
         <v>43811</v>
       </c>
       <c r="E229" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="I229" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="230" spans="1:9">
@@ -6586,7 +6602,7 @@
         <v>43812.713796296295</v>
       </c>
       <c r="B230" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C230" t="s">
         <v>16</v>
@@ -6596,7 +6612,7 @@
       </c>
       <c r="E230" s="2"/>
       <c r="F230" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="231" spans="1:9">
@@ -6614,7 +6630,7 @@
       </c>
       <c r="E231" s="2"/>
       <c r="I231" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="232" spans="1:9">
@@ -6632,10 +6648,10 @@
       </c>
       <c r="E232" s="2"/>
       <c r="I232" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="233" spans="1:9">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="233" spans="1:9" ht="17.25" customHeight="1">
       <c r="A233" s="1">
         <v>43817.92465277778</v>
       </c>
@@ -6649,8 +6665,8 @@
         <v>43748</v>
       </c>
       <c r="E233" s="2"/>
-      <c r="F233" t="s">
-        <v>256</v>
+      <c r="F233" s="15" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="234" spans="1:9">
@@ -6667,10 +6683,10 @@
         <v>43790</v>
       </c>
       <c r="E234" s="5" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="I234" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="235" spans="1:9">
@@ -6691,7 +6707,7 @@
         <v>1</v>
       </c>
       <c r="I235" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="236" spans="1:9">
@@ -6699,7 +6715,7 @@
         <v>43833.66547453704</v>
       </c>
       <c r="B236" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C236" t="s">
         <v>28</v>
@@ -6708,10 +6724,10 @@
         <v>43832</v>
       </c>
       <c r="E236" s="5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="I236" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="237" spans="1:9">
@@ -6728,10 +6744,10 @@
         <v>43767</v>
       </c>
       <c r="E237" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I237" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="238" spans="1:9">
@@ -6752,7 +6768,7 @@
         <v>60</v>
       </c>
       <c r="I238" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="239" spans="1:9">
@@ -6773,7 +6789,7 @@
         <v>50</v>
       </c>
       <c r="I239" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="240" spans="1:9">
@@ -6794,7 +6810,7 @@
         <v>40</v>
       </c>
       <c r="I240" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="241" spans="1:9">
@@ -6815,7 +6831,7 @@
         <v>22</v>
       </c>
       <c r="I241" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="242" spans="1:9">
@@ -6836,7 +6852,7 @@
         <v>1</v>
       </c>
       <c r="I242" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="243" spans="1:9">
@@ -6857,7 +6873,7 @@
         <v>20</v>
       </c>
       <c r="I243" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="244" spans="1:9">
@@ -6878,7 +6894,7 @@
         <v>16</v>
       </c>
       <c r="I244" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="245" spans="1:9">
@@ -6886,7 +6902,7 @@
         <v>43836.690509259257</v>
       </c>
       <c r="B245" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C245" t="s">
         <v>12</v>
@@ -6899,7 +6915,7 @@
         <v>1</v>
       </c>
       <c r="I245" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="246" spans="1:9">
@@ -6907,7 +6923,7 @@
         <v>43836.691168981481</v>
       </c>
       <c r="B246" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C246" t="s">
         <v>10</v>
@@ -6920,7 +6936,7 @@
         <v>2</v>
       </c>
       <c r="I246" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="247" spans="1:9">
@@ -6937,13 +6953,13 @@
         <v>43838</v>
       </c>
       <c r="E247" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G247">
         <v>50</v>
       </c>
       <c r="I247" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="248" spans="1:9">
@@ -6964,7 +6980,7 @@
         <v>15</v>
       </c>
       <c r="I248" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="249" spans="1:9">
@@ -6982,7 +6998,7 @@
       </c>
       <c r="E249" s="2"/>
       <c r="F249" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="250" spans="1:9">
@@ -7003,7 +7019,7 @@
         <v>125</v>
       </c>
       <c r="I250" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="251" spans="1:9">
@@ -7024,7 +7040,7 @@
         <v>50</v>
       </c>
       <c r="I251" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="252" spans="1:9">
@@ -7045,7 +7061,7 @@
         <v>7</v>
       </c>
       <c r="I252" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="253" spans="1:9">
@@ -7066,7 +7082,7 @@
         <v>7</v>
       </c>
       <c r="I253" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="254" spans="1:9">
@@ -7084,7 +7100,7 @@
       </c>
       <c r="E254" s="2"/>
       <c r="I254" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="255" spans="1:9">
@@ -7102,7 +7118,7 @@
       </c>
       <c r="E255" s="2"/>
       <c r="F255" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="256" spans="1:9">
@@ -7120,7 +7136,7 @@
       </c>
       <c r="E256" s="2"/>
       <c r="I256" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="257" spans="1:9">
@@ -7144,7 +7160,7 @@
         <v>1</v>
       </c>
       <c r="I257" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="258" spans="1:9">
@@ -7177,10 +7193,10 @@
       </c>
       <c r="E259" s="2"/>
       <c r="F259" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="I259" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="260" spans="1:9">
@@ -7198,7 +7214,7 @@
       </c>
       <c r="E260" s="2"/>
       <c r="I260" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="261" spans="1:9">
@@ -7216,7 +7232,7 @@
       </c>
       <c r="E261" s="2"/>
       <c r="F261" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="262" spans="1:9">
@@ -7224,7 +7240,7 @@
         <v>43899.822476851848</v>
       </c>
       <c r="B262" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C262" t="s">
         <v>16</v>
@@ -7232,12 +7248,14 @@
       <c r="D262" s="2">
         <v>43836</v>
       </c>
-      <c r="E262" s="2"/>
+      <c r="E262" s="13" t="s">
+        <v>290</v>
+      </c>
       <c r="F262" s="5" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="I262" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="263" spans="1:9">
@@ -7245,7 +7263,7 @@
         <v>43899.823437500003</v>
       </c>
       <c r="B263" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C263" t="s">
         <v>12</v>
@@ -7255,7 +7273,7 @@
       </c>
       <c r="E263" s="2"/>
       <c r="I263" s="5" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="264" spans="1:9">
@@ -7263,7 +7281,7 @@
         <v>43899.824756944443</v>
       </c>
       <c r="B264" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C264" t="s">
         <v>10</v>
@@ -7276,7 +7294,7 @@
         <v>14</v>
       </c>
       <c r="I264" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="265" spans="1:9">
@@ -7284,7 +7302,7 @@
         <v>43899.825312499997</v>
       </c>
       <c r="B265" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C265" t="s">
         <v>12</v>
@@ -7294,7 +7312,7 @@
       </c>
       <c r="E265" s="2"/>
       <c r="I265" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="266" spans="1:9">
@@ -7302,7 +7320,7 @@
         <v>43899.825694444444</v>
       </c>
       <c r="B266" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C266" t="s">
         <v>12</v>
@@ -7312,7 +7330,7 @@
       </c>
       <c r="E266" s="2"/>
       <c r="I266" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="267" spans="1:9">
@@ -7320,7 +7338,7 @@
         <v>43899.826585648145</v>
       </c>
       <c r="B267" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C267" t="s">
         <v>12</v>
@@ -7329,10 +7347,10 @@
         <v>43872</v>
       </c>
       <c r="E267" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="I267" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="268" spans="1:9">
@@ -7340,7 +7358,7 @@
         <v>43899.827326388891</v>
       </c>
       <c r="B268" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C268" t="s">
         <v>12</v>
@@ -7349,10 +7367,10 @@
         <v>43873</v>
       </c>
       <c r="E268" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="I268" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="269" spans="1:9">
@@ -7360,7 +7378,7 @@
         <v>43899.827893518515</v>
       </c>
       <c r="B269" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C269" t="s">
         <v>12</v>
@@ -7370,7 +7388,7 @@
       </c>
       <c r="E269" s="2"/>
       <c r="I269" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="270" spans="1:9">
@@ -7378,7 +7396,7 @@
         <v>43899.828194444446</v>
       </c>
       <c r="B270" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C270" t="s">
         <v>12</v>
@@ -7388,7 +7406,7 @@
       </c>
       <c r="E270" s="2"/>
       <c r="I270" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="271" spans="1:9">
@@ -7396,7 +7414,7 @@
         <v>43899.828761574077</v>
       </c>
       <c r="B271" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C271" t="s">
         <v>12</v>
@@ -7406,7 +7424,7 @@
       </c>
       <c r="E271" s="2"/>
       <c r="I271" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="272" spans="1:9">
@@ -7414,7 +7432,7 @@
         <v>43899.831238425926</v>
       </c>
       <c r="B272" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C272" t="s">
         <v>28</v>
@@ -7423,10 +7441,10 @@
         <v>43854</v>
       </c>
       <c r="E272" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="I272" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="273" spans="1:9">
@@ -7434,7 +7452,7 @@
         <v>43899.832048611112</v>
       </c>
       <c r="B273" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C273" t="s">
         <v>28</v>
@@ -7443,10 +7461,10 @@
         <v>43867</v>
       </c>
       <c r="E273" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="I273" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="274" spans="1:9">
@@ -7454,7 +7472,7 @@
         <v>43899.832395833335</v>
       </c>
       <c r="B274" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C274" t="s">
         <v>28</v>
@@ -7463,10 +7481,10 @@
         <v>43840</v>
       </c>
       <c r="E274" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="I274" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="275" spans="1:9">
@@ -7474,7 +7492,7 @@
         <v>43899.833009259259</v>
       </c>
       <c r="B275" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C275" t="s">
         <v>28</v>
@@ -7483,10 +7501,10 @@
         <v>43837</v>
       </c>
       <c r="E275" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="I275" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="276" spans="1:9">
@@ -7494,7 +7512,7 @@
         <v>43899.83353009259</v>
       </c>
       <c r="B276" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C276" t="s">
         <v>28</v>
@@ -7503,10 +7521,10 @@
         <v>43836</v>
       </c>
       <c r="E276" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="I276" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="277" spans="1:9">
@@ -7527,7 +7545,7 @@
         <v>25</v>
       </c>
       <c r="I277" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="278" spans="1:9">
@@ -7545,7 +7563,7 @@
       </c>
       <c r="E278" s="2"/>
       <c r="I278" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="279" spans="1:9">
@@ -7566,7 +7584,7 @@
         <v>12</v>
       </c>
       <c r="I279" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="280" spans="1:9">
@@ -7574,7 +7592,7 @@
         <v>43921.718981481485</v>
       </c>
       <c r="B280" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C280" t="s">
         <v>12</v>
@@ -7584,7 +7602,7 @@
       </c>
       <c r="E280" s="2"/>
       <c r="I280" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="281" spans="1:9">
@@ -7592,7 +7610,7 @@
         <v>43921.719467592593</v>
       </c>
       <c r="B281" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C281" t="s">
         <v>12</v>
@@ -7602,7 +7620,7 @@
       </c>
       <c r="E281" s="2"/>
       <c r="I281" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
     <row r="282" spans="1:9">
@@ -7610,7 +7628,7 @@
         <v>43921.720173611109</v>
       </c>
       <c r="B282" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C282" t="s">
         <v>12</v>
@@ -7620,7 +7638,7 @@
       </c>
       <c r="E282" s="2"/>
       <c r="I282" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="283" spans="1:9">
@@ -7628,7 +7646,7 @@
         <v>43921.721006944441</v>
       </c>
       <c r="B283" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C283" t="s">
         <v>10</v>
@@ -7641,7 +7659,7 @@
         <v>9</v>
       </c>
       <c r="I283" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="284" spans="1:9">
@@ -7658,10 +7676,10 @@
         <v>43852</v>
       </c>
       <c r="E284" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="I284" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="285" spans="1:9">
@@ -7679,7 +7697,7 @@
       </c>
       <c r="E285" s="2"/>
       <c r="I285" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="286" spans="1:9">
@@ -7697,7 +7715,7 @@
       </c>
       <c r="E286" s="2"/>
       <c r="I286" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="287" spans="1:9">
@@ -7715,7 +7733,7 @@
       </c>
       <c r="E287" s="2"/>
       <c r="I287" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="288" spans="1:9">
@@ -7736,7 +7754,7 @@
         <v>1</v>
       </c>
       <c r="I288" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="289" spans="1:9">
@@ -7757,7 +7775,7 @@
         <v>5</v>
       </c>
       <c r="I289" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="290" spans="1:9">
@@ -7778,7 +7796,7 @@
         <v>25</v>
       </c>
       <c r="I290" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="291" spans="1:9">
@@ -7799,7 +7817,7 @@
         <v>34</v>
       </c>
       <c r="I291" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="292" spans="1:9">
@@ -7807,7 +7825,7 @@
         <v>43923.79215277778</v>
       </c>
       <c r="B292" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C292" t="s">
         <v>12</v>
@@ -7820,7 +7838,7 @@
         <v>20</v>
       </c>
       <c r="I292" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="293" spans="1:9">
@@ -7828,7 +7846,7 @@
         <v>43923.79310185185</v>
       </c>
       <c r="B293" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C293" t="s">
         <v>20</v>
@@ -7837,10 +7855,10 @@
         <v>43881</v>
       </c>
       <c r="E293" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="I293" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="294" spans="1:9">
@@ -7848,7 +7866,7 @@
         <v>43923.79383101852</v>
       </c>
       <c r="B294" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C294" t="s">
         <v>20</v>
@@ -7857,10 +7875,10 @@
         <v>43893</v>
       </c>
       <c r="E294" s="5" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="I294" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="295" spans="1:9">
@@ -7868,7 +7886,7 @@
         <v>43923.794479166667</v>
       </c>
       <c r="B295" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C295" t="s">
         <v>12</v>
@@ -7881,7 +7899,7 @@
         <v>4</v>
       </c>
       <c r="I295" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="296" spans="1:9">
@@ -7889,7 +7907,7 @@
         <v>43923.795162037037</v>
       </c>
       <c r="B296" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C296" t="s">
         <v>10</v>
@@ -7902,7 +7920,7 @@
         <v>1</v>
       </c>
       <c r="I296" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="297" spans="1:9">
@@ -7910,7 +7928,7 @@
         <v>43923.795844907407</v>
       </c>
       <c r="B297" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C297" t="s">
         <v>10</v>
@@ -7923,7 +7941,7 @@
         <v>1</v>
       </c>
       <c r="I297" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="298" spans="1:9">
@@ -7944,7 +7962,7 @@
         <v>15</v>
       </c>
       <c r="I298" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
     </row>
     <row r="299" spans="1:9">
@@ -7962,10 +7980,10 @@
       </c>
       <c r="E299" s="2"/>
       <c r="G299" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="I299" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="300" spans="1:9">
@@ -7986,7 +8004,7 @@
         <v>8</v>
       </c>
       <c r="I300" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="301" spans="1:9">
@@ -8004,7 +8022,7 @@
       </c>
       <c r="E301" s="2"/>
       <c r="F301" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="302" spans="1:9">
@@ -8025,7 +8043,7 @@
         <v>12</v>
       </c>
       <c r="I302" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
     <row r="303" spans="1:9">
@@ -8046,7 +8064,7 @@
         <v>100</v>
       </c>
       <c r="I303" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="304" spans="1:9">
@@ -8064,7 +8082,7 @@
       </c>
       <c r="E304" s="2"/>
       <c r="I304" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
     </row>
     <row r="305" spans="1:9">
@@ -8082,7 +8100,7 @@
       </c>
       <c r="E305" s="2"/>
       <c r="F305" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="306" spans="1:9">
@@ -8103,7 +8121,7 @@
         <v>18</v>
       </c>
       <c r="I306" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
     </row>
     <row r="307" spans="1:9">
@@ -8111,7 +8129,7 @@
         <v>43928.746782407405</v>
       </c>
       <c r="B307" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C307" t="s">
         <v>20</v>
@@ -8127,7 +8145,7 @@
         <v>484</v>
       </c>
       <c r="I307" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="308" spans="1:9">
@@ -8135,7 +8153,7 @@
         <v>43928.752442129633</v>
       </c>
       <c r="B308" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C308" t="s">
         <v>20</v>
@@ -8148,7 +8166,7 @@
         <v>1</v>
       </c>
       <c r="I308" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
     </row>
     <row r="309" spans="1:9">
@@ -8169,7 +8187,7 @@
         <v>2</v>
       </c>
       <c r="I309" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="310" spans="1:9">
@@ -8187,7 +8205,7 @@
       </c>
       <c r="E310" s="2"/>
       <c r="I310" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
     <row r="311" spans="1:9">
@@ -8205,7 +8223,7 @@
       </c>
       <c r="E311" s="2"/>
       <c r="I311" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="312" spans="1:9">
@@ -8223,7 +8241,7 @@
       </c>
       <c r="E312" s="2"/>
       <c r="I312" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="313" spans="1:9">
@@ -8231,7 +8249,7 @@
         <v>43956.726342592592</v>
       </c>
       <c r="B313" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="C313" t="s">
         <v>12</v>
@@ -8241,7 +8259,7 @@
       </c>
       <c r="E313" s="2"/>
       <c r="I313" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="314" spans="1:9">
@@ -8259,7 +8277,7 @@
       </c>
       <c r="E314" s="2"/>
       <c r="I314" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="315" spans="1:9">
@@ -8277,7 +8295,7 @@
       </c>
       <c r="E315" s="2"/>
       <c r="I315" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="316" spans="1:9">
@@ -8285,7 +8303,7 @@
         <v>43963.709398148145</v>
       </c>
       <c r="B316" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C316" t="s">
         <v>12</v>
@@ -8295,7 +8313,7 @@
       </c>
       <c r="E316" s="2"/>
       <c r="I316" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="317" spans="1:9">
@@ -8303,7 +8321,7 @@
         <v>43963.712002314816</v>
       </c>
       <c r="B317" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C317" t="s">
         <v>20</v>
@@ -8319,7 +8337,7 @@
         <v>420</v>
       </c>
       <c r="I317" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
     </row>
     <row r="318" spans="1:9">
@@ -8327,7 +8345,7 @@
         <v>43963.759155092594</v>
       </c>
       <c r="B318" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C318" t="s">
         <v>20</v>
@@ -8343,7 +8361,7 @@
         <v>21</v>
       </c>
       <c r="I318" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="319" spans="1:9">
@@ -8361,7 +8379,7 @@
       </c>
       <c r="E319" s="2"/>
       <c r="I319" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
     </row>
     <row r="320" spans="1:9">
@@ -8379,7 +8397,7 @@
       </c>
       <c r="E320" s="2"/>
       <c r="I320" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="321" spans="1:9">
@@ -8396,10 +8414,10 @@
         <v>43976</v>
       </c>
       <c r="E321" s="2" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="I321" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="322" spans="1:9">
@@ -8423,7 +8441,7 @@
         <v>480</v>
       </c>
       <c r="I322" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="323" spans="1:9">
@@ -8441,7 +8459,7 @@
       </c>
       <c r="E323" s="2"/>
       <c r="I323" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
     </row>
     <row r="324" spans="1:9">
@@ -8459,7 +8477,7 @@
       </c>
       <c r="E324" s="2"/>
       <c r="I324" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="325" spans="1:9">
@@ -8476,10 +8494,10 @@
         <v>43986</v>
       </c>
       <c r="E325" s="2" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="I325" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row r="326" spans="1:9">
@@ -8487,7 +8505,7 @@
         <v>43993.69699074074</v>
       </c>
       <c r="B326" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C326" t="s">
         <v>16</v>
@@ -8496,10 +8514,10 @@
         <v>43923</v>
       </c>
       <c r="E326" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="F326" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="327" spans="1:9">
@@ -8517,7 +8535,7 @@
       </c>
       <c r="E327" s="2"/>
       <c r="I327" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
     </row>
     <row r="328" spans="1:9">
@@ -8534,10 +8552,10 @@
         <v>44004</v>
       </c>
       <c r="E328" s="13" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="I328" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
     </row>
     <row r="329" spans="1:9">
@@ -8554,10 +8572,10 @@
         <v>43972</v>
       </c>
       <c r="E329" s="2" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="F329" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
     </row>
     <row r="330" spans="1:9">
@@ -8575,7 +8593,7 @@
       </c>
       <c r="E330" s="2"/>
       <c r="I330" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="331" spans="1:9">
@@ -8593,7 +8611,7 @@
       </c>
       <c r="E331" s="2"/>
       <c r="I331" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
     </row>
     <row r="332" spans="1:9">
@@ -8610,10 +8628,10 @@
         <v>43955</v>
       </c>
       <c r="E332" s="2" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="F332" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
     <row r="333" spans="1:9">
@@ -8630,10 +8648,10 @@
         <v>43993</v>
       </c>
       <c r="E333" s="2" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="F333" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
     </row>
     <row r="334" spans="1:9">
@@ -8650,10 +8668,10 @@
         <v>43955</v>
       </c>
       <c r="E334" s="2" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="I334" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
     </row>
     <row r="335" spans="1:9">
@@ -8674,7 +8692,7 @@
         <v>10</v>
       </c>
       <c r="I335" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
     <row r="336" spans="1:9">
@@ -8695,7 +8713,7 @@
         <v>510</v>
       </c>
       <c r="I336" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
     </row>
     <row r="337" spans="1:9">
@@ -8712,10 +8730,10 @@
         <v>44000</v>
       </c>
       <c r="E337" s="2" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="I337" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="338" spans="1:9">
@@ -8736,7 +8754,7 @@
         <v>6</v>
       </c>
       <c r="I338" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
     </row>
     <row r="339" spans="1:9">
@@ -8757,7 +8775,7 @@
         <v>10</v>
       </c>
       <c r="I339" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
     </row>
     <row r="340" spans="1:9">
@@ -8774,10 +8792,10 @@
         <v>43986</v>
       </c>
       <c r="E340" s="2" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="F340" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
     </row>
     <row r="341" spans="1:9">
@@ -8801,7 +8819,7 @@
         <v>50</v>
       </c>
       <c r="I341" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
     </row>
     <row r="342" spans="1:9">
@@ -8825,7 +8843,7 @@
         <v>304</v>
       </c>
       <c r="I342" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
     </row>
     <row r="343" spans="1:9">
@@ -8833,7 +8851,7 @@
         <v>44034.844490740739</v>
       </c>
       <c r="B343" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C343" t="s">
         <v>28</v>
@@ -8842,7 +8860,7 @@
         <v>43927</v>
       </c>
       <c r="E343" s="2" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="344" spans="1:9">
@@ -8850,7 +8868,7 @@
         <v>44034.845335648148</v>
       </c>
       <c r="B344" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C344" t="s">
         <v>10</v>
@@ -8863,7 +8881,7 @@
         <v>13</v>
       </c>
       <c r="I344" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
     </row>
     <row r="345" spans="1:9">
@@ -8871,7 +8889,7 @@
         <v>44034.853518518517</v>
       </c>
       <c r="B345" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C345" t="s">
         <v>20</v>
@@ -8887,7 +8905,7 @@
         <v>2</v>
       </c>
       <c r="I345" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
     </row>
     <row r="346" spans="1:9">
@@ -8905,7 +8923,7 @@
       </c>
       <c r="E346" s="2"/>
       <c r="I346" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
     </row>
     <row r="347" spans="1:9">
@@ -8923,7 +8941,7 @@
       </c>
       <c r="E347" s="2"/>
       <c r="I347" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="348" spans="1:9">
@@ -8941,7 +8959,7 @@
       </c>
       <c r="E348" s="2"/>
       <c r="I348" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
     </row>
     <row r="349" spans="1:9">
@@ -8958,10 +8976,10 @@
         <v>43983</v>
       </c>
       <c r="E349" s="13" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F349" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
     </row>
     <row r="350" spans="1:9">
@@ -8978,10 +8996,10 @@
         <v>43952</v>
       </c>
       <c r="E350" s="13" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="F350" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="351" spans="1:9">
@@ -8998,10 +9016,10 @@
         <v>44031</v>
       </c>
       <c r="E351" s="13" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="F351" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
     </row>
     <row r="352" spans="1:9">
@@ -9025,7 +9043,7 @@
         <v>56</v>
       </c>
       <c r="I352" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
     </row>
     <row r="353" spans="1:9">
@@ -9046,7 +9064,7 @@
         <v>1</v>
       </c>
       <c r="I353" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
     </row>
     <row r="354" spans="1:9">
@@ -9067,7 +9085,7 @@
         <v>1</v>
       </c>
       <c r="I354" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
     </row>
     <row r="355" spans="1:9">
@@ -9084,10 +9102,10 @@
         <v>44040</v>
       </c>
       <c r="E355" s="13" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I355" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
     </row>
     <row r="356" spans="1:9">
@@ -9104,10 +9122,10 @@
         <v>44042</v>
       </c>
       <c r="E356" s="13" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="I356" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
     </row>
     <row r="357" spans="1:9">
@@ -9124,10 +9142,10 @@
         <v>44040</v>
       </c>
       <c r="E357" s="13" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="F357" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
     </row>
     <row r="358" spans="1:9">
@@ -9144,10 +9162,10 @@
         <v>44043</v>
       </c>
       <c r="E358" s="13" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="I358" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
     </row>
     <row r="359" spans="1:9">
@@ -9164,10 +9182,10 @@
         <v>44046</v>
       </c>
       <c r="E359" s="13" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="I359" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
     </row>
     <row r="360" spans="1:9">
@@ -9184,10 +9202,10 @@
         <v>44040</v>
       </c>
       <c r="E360" s="13" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="I360" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
     </row>
     <row r="361" spans="1:9">
@@ -9204,10 +9222,10 @@
         <v>44046</v>
       </c>
       <c r="E361" s="13" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="I361" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
     </row>
     <row r="362" spans="1:9">
@@ -9224,10 +9242,10 @@
         <v>44047</v>
       </c>
       <c r="E362" s="13" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="I362" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
     </row>
     <row r="363" spans="1:9">
@@ -9235,7 +9253,7 @@
         <v>44053.67465277778</v>
       </c>
       <c r="B363" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C363" t="s">
         <v>16</v>
@@ -9244,10 +9262,10 @@
         <v>44052</v>
       </c>
       <c r="E363" s="13" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="F363" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
     </row>
     <row r="364" spans="1:9">
@@ -9255,7 +9273,7 @@
         <v>44053.679502314815</v>
       </c>
       <c r="B364" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C364" t="s">
         <v>10</v>
@@ -9268,7 +9286,7 @@
         <v>1</v>
       </c>
       <c r="I364" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
     </row>
     <row r="365" spans="1:9">
@@ -9276,7 +9294,7 @@
         <v>44053.6797337963</v>
       </c>
       <c r="B365" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C365" t="s">
         <v>10</v>
@@ -9289,7 +9307,7 @@
         <v>1</v>
       </c>
       <c r="I365" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
     </row>
     <row r="366" spans="1:9">
@@ -9297,7 +9315,7 @@
         <v>44053.679930555554</v>
       </c>
       <c r="B366" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C366" t="s">
         <v>10</v>
@@ -9310,7 +9328,7 @@
         <v>1</v>
       </c>
       <c r="I366" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
     </row>
     <row r="367" spans="1:9">
@@ -9318,7 +9336,7 @@
         <v>44053.680312500001</v>
       </c>
       <c r="B367" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C367" t="s">
         <v>10</v>
@@ -9331,7 +9349,7 @@
         <v>3</v>
       </c>
       <c r="I367" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
     <row r="368" spans="1:9">
@@ -9348,10 +9366,10 @@
         <v>44002</v>
       </c>
       <c r="E368" s="13" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="F368" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
     <row r="369" spans="1:9">
@@ -9372,7 +9390,7 @@
         <v>21</v>
       </c>
       <c r="I369" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
     </row>
     <row r="370" spans="1:9">
@@ -9396,7 +9414,7 @@
         <v>800</v>
       </c>
       <c r="I370" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
     </row>
     <row r="371" spans="1:9">
@@ -9413,10 +9431,10 @@
         <v>44053</v>
       </c>
       <c r="E371" s="13" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="I371" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
     </row>
     <row r="372" spans="1:9">
@@ -9433,10 +9451,10 @@
         <v>44058</v>
       </c>
       <c r="E372" s="13" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="I372" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
     </row>
     <row r="373" spans="1:9">
@@ -9457,7 +9475,7 @@
         <v>8</v>
       </c>
       <c r="I373" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
     <row r="374" spans="1:9">
@@ -9474,10 +9492,10 @@
         <v>44056</v>
       </c>
       <c r="E374" s="13" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="I374" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
     </row>
     <row r="375" spans="1:9">
@@ -9495,7 +9513,7 @@
       </c>
       <c r="E375" s="13"/>
       <c r="I375" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
     </row>
     <row r="376" spans="1:9">
@@ -9516,7 +9534,7 @@
         <v>3</v>
       </c>
       <c r="I376" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
     </row>
     <row r="377" spans="1:9">
@@ -9537,7 +9555,7 @@
         <v>3</v>
       </c>
       <c r="I377" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="378" spans="1:9">
@@ -9561,7 +9579,7 @@
         <v>14</v>
       </c>
       <c r="I378" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
     </row>
     <row r="379" spans="1:9">
@@ -9569,7 +9587,7 @@
         <v>44071.626631944448</v>
       </c>
       <c r="B379" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C379" t="s">
         <v>28</v>
@@ -9578,10 +9596,30 @@
         <v>44067</v>
       </c>
       <c r="E379" s="13" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="I379" t="s">
-        <v>443</v>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="380" spans="1:9">
+      <c r="A380" s="1">
+        <v>44071.626631944448</v>
+      </c>
+      <c r="B380" t="s">
+        <v>19</v>
+      </c>
+      <c r="C380" t="s">
+        <v>16</v>
+      </c>
+      <c r="D380" s="2">
+        <v>43800</v>
+      </c>
+      <c r="E380" s="13" t="s">
+        <v>446</v>
+      </c>
+      <c r="F380" t="s">
+        <v>447</v>
       </c>
     </row>
   </sheetData>
@@ -9600,21 +9638,23 @@
     <hyperlink ref="E236" r:id="rId12" xr:uid="{863BC4B1-6351-418B-B98F-87ECBB33C30C}"/>
     <hyperlink ref="E150" r:id="rId13" xr:uid="{E6C2CF85-2279-490C-9FF0-B2F4FFAF65F5}"/>
     <hyperlink ref="E151" r:id="rId14" xr:uid="{3537EE39-869F-4C8C-AD1E-522F607F66F5}"/>
-    <hyperlink ref="F262" r:id="rId15" display="https://www.pnas.org/content/117/3/1587.short   Recovery of critically endangered Nassau grouper (Epinephelus striatus) in the Cayman Islands following targeted conservation actions Lynn Waterhouse, Scott A. Heppell, Christy V. Pattengill-Semmens, Croy McCoy, Phillippe Bush, Bradley C. Johnson, Brice X. Semmens Proceedings of the National Academy of Sciences Jan 2020, 117 (3) 1587-1595; DOI: 10.1073/pnas.1917132117" xr:uid="{99A0F466-A75A-4E4E-A6F4-620C55E4BC39}"/>
-    <hyperlink ref="E294" r:id="rId16" xr:uid="{783C5FCB-679F-4B9C-825F-6DEF83E5F389}"/>
-    <hyperlink ref="I263" r:id="rId17" xr:uid="{B2F6CA54-1A89-4AF4-81AE-0F5BB3E65DE4}"/>
-    <hyperlink ref="E226" r:id="rId18" xr:uid="{3137DA4B-211F-4BEA-9B82-14FC40BD36B0}"/>
-    <hyperlink ref="E350" r:id="rId19" xr:uid="{27099907-A031-4B65-A453-522A3713C9C5}"/>
-    <hyperlink ref="E349" r:id="rId20" xr:uid="{05BDD9DB-8015-4AB0-A9C6-AB83241EE286}"/>
-    <hyperlink ref="E357" r:id="rId21" xr:uid="{4B576F19-3DA3-4771-B241-816AB98BEFCA}"/>
-    <hyperlink ref="E363" r:id="rId22" location="citeas" xr:uid="{B046AA8A-1960-4984-86A2-4DBE219428F2}"/>
-    <hyperlink ref="E371" r:id="rId23" xr:uid="{C085667D-D3C4-410D-8CD0-8C9B000220F7}"/>
-    <hyperlink ref="E328" r:id="rId24" xr:uid="{5E022E0D-F407-4392-8F4A-7810D15676C1}"/>
+    <hyperlink ref="E294" r:id="rId15" xr:uid="{783C5FCB-679F-4B9C-825F-6DEF83E5F389}"/>
+    <hyperlink ref="I263" r:id="rId16" xr:uid="{B2F6CA54-1A89-4AF4-81AE-0F5BB3E65DE4}"/>
+    <hyperlink ref="E226" r:id="rId17" xr:uid="{3137DA4B-211F-4BEA-9B82-14FC40BD36B0}"/>
+    <hyperlink ref="E350" r:id="rId18" xr:uid="{27099907-A031-4B65-A453-522A3713C9C5}"/>
+    <hyperlink ref="E349" r:id="rId19" xr:uid="{05BDD9DB-8015-4AB0-A9C6-AB83241EE286}"/>
+    <hyperlink ref="E357" r:id="rId20" xr:uid="{4B576F19-3DA3-4771-B241-816AB98BEFCA}"/>
+    <hyperlink ref="E363" r:id="rId21" location="citeas" xr:uid="{B046AA8A-1960-4984-86A2-4DBE219428F2}"/>
+    <hyperlink ref="E371" r:id="rId22" xr:uid="{C085667D-D3C4-410D-8CD0-8C9B000220F7}"/>
+    <hyperlink ref="E328" r:id="rId23" xr:uid="{5E022E0D-F407-4392-8F4A-7810D15676C1}"/>
+    <hyperlink ref="E98" r:id="rId24" xr:uid="{641B07AD-3328-4D02-A3D6-401C24AEB3A4}"/>
+    <hyperlink ref="E380" r:id="rId25" xr:uid="{96BE78CA-5236-4631-A9C5-0A4075396DFA}"/>
+    <hyperlink ref="E262" r:id="rId26" xr:uid="{A9D8A46F-4623-45DA-9892-E087A0E85158}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId25"/>
+  <legacyDrawing r:id="rId27"/>
   <tableParts count="1">
-    <tablePart r:id="rId26"/>
+    <tablePart r:id="rId28"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>